<commit_message>
remove *-base-type leaf, adapt script to new .sid format
</commit_message>
<xml_diff>
--- a/SID-mapping.xlsx
+++ b/SID-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae8058082ac65dd3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/Library/CloudStorage/OneDrive-Personnel/Documents/xlapak/schc-wg/YANG-DM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD9A47F2-96B8-4D81-89A0-1AF1FF614C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67D388F6-B909-F847-94A8-B20754F36085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="12160" windowWidth="47160" windowHeight="25720" xr2:uid="{79CBBA98-45D0-AB4B-8F46-38D859212AB5}"/>
+    <workbookView xWindow="4040" yWindow="1060" windowWidth="47160" windowHeight="25720" xr2:uid="{79CBBA98-45D0-AB4B-8F46-38D859212AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="SID Allocation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="155">
   <si>
     <t>module</t>
   </si>
@@ -499,13 +499,16 @@
   </si>
   <si>
     <t>fid-coap-option-uri-query</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This option overload universal-option to add hierarchy in typing, the rule should not use it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -899,153 +902,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE7973-9DF4-B240-B0AB-F84379B61AEA}">
   <dimension ref="A1:E400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="F379" sqref="F379"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2550</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>A1+1</f>
         <v>2551</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>2552</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2553</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>2554</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>2555</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2556</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>2557</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>2558</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>2559</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>2560</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>2561</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>2562</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>2563</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>2564</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>2565</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>2566</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>2567</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>2568</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>2569</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>2570</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>2571</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>2572</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>2573</v>
@@ -1060,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>2574</v>
@@ -1072,139 +1075,139 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>2575</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>2576</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>2577</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>2578</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>2579</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>2580</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>2581</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>2582</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>2583</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>2584</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>2585</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>2586</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>2587</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>2588</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
         <v>2589</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
         <v>2591</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
         <v>2592</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
         <v>2593</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
         <v>2594</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <f t="shared" si="0"/>
         <v>2595</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <f t="shared" si="0"/>
         <v>2596</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>2597</v>
@@ -1219,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>2598</v>
@@ -1237,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>2599</v>
@@ -1255,7 +1258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>2600</v>
@@ -1273,13 +1276,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>2601</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>2602</v>
@@ -1288,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>2603</v>
@@ -1297,7 +1300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>2604</v>
@@ -1306,7 +1309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>2605</v>
@@ -1315,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>2606</v>
@@ -1324,7 +1327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>2607</v>
@@ -1333,7 +1336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>2608</v>
@@ -1342,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>2609</v>
@@ -1351,7 +1354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>2610</v>
@@ -1360,7 +1363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>2611</v>
@@ -1369,7 +1372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>2612</v>
@@ -1378,7 +1381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>2613</v>
@@ -1387,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>2614</v>
@@ -1396,7 +1399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>2615</v>
@@ -1405,7 +1408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <f t="shared" ref="A67:A130" si="1">A66+1</f>
         <v>2616</v>
@@ -1414,7 +1417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <f t="shared" si="1"/>
         <v>2617</v>
@@ -1423,7 +1426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <f t="shared" si="1"/>
         <v>2618</v>
@@ -1432,13 +1435,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
         <v>2619</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="D70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <f t="shared" si="1"/>
         <v>2620</v>
@@ -1456,7 +1462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <f t="shared" si="1"/>
         <v>2621</v>
@@ -1474,7 +1480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <f t="shared" si="1"/>
         <v>2622</v>
@@ -1492,7 +1498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <f t="shared" si="1"/>
         <v>2623</v>
@@ -1510,7 +1516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <f t="shared" si="1"/>
         <v>2624</v>
@@ -1528,7 +1534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <f t="shared" si="1"/>
         <v>2625</v>
@@ -1546,7 +1552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <f t="shared" si="1"/>
         <v>2626</v>
@@ -1564,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <f t="shared" si="1"/>
         <v>2627</v>
@@ -1582,7 +1588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
         <v>2628</v>
@@ -1600,7 +1606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
         <v>2629</v>
@@ -1618,7 +1624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
         <v>2630</v>
@@ -1636,7 +1642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
         <v>2631</v>
@@ -1654,7 +1660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
         <v>2632</v>
@@ -1672,7 +1678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <f t="shared" si="1"/>
         <v>2633</v>
@@ -1690,7 +1696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <f t="shared" si="1"/>
         <v>2634</v>
@@ -1708,7 +1714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <f t="shared" si="1"/>
         <v>2635</v>
@@ -1726,55 +1732,55 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <f t="shared" si="1"/>
         <v>2636</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <f t="shared" si="1"/>
         <v>2637</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <f t="shared" si="1"/>
         <v>2638</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <f t="shared" si="1"/>
         <v>2639</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <f t="shared" si="1"/>
         <v>2640</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <f t="shared" si="1"/>
         <v>2641</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <f t="shared" si="1"/>
         <v>2642</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <f t="shared" si="1"/>
         <v>2643</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>2644</v>
@@ -1789,7 +1795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>2645</v>
@@ -1804,7 +1810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>2646</v>
@@ -1819,7 +1825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>2647</v>
@@ -1834,7 +1840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>2648</v>
@@ -1849,7 +1855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>2649</v>
@@ -1864,7 +1870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>2650</v>
@@ -1879,7 +1885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>2651</v>
@@ -1894,7 +1900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>2652</v>
@@ -1909,7 +1915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>2653</v>
@@ -1924,7 +1930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>2654</v>
@@ -1939,7 +1945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>2655</v>
@@ -1954,7 +1960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>2656</v>
@@ -1969,7 +1975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>2657</v>
@@ -1984,7 +1990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>2658</v>
@@ -1999,7 +2005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>2659</v>
@@ -2014,7 +2020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>2660</v>
@@ -2029,7 +2035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>2661</v>
@@ -2044,7 +2050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>2662</v>
@@ -2059,7 +2065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>2663</v>
@@ -2074,7 +2080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>2664</v>
@@ -2083,37 +2089,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>2665</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>2666</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>2667</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>2668</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>2669</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>2670</v>
@@ -2122,811 +2128,811 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>2671</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>2672</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>2673</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>2674</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>2675</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>2676</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>2677</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>2678</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>2679</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" ref="A131:A194" si="2">A130+1</f>
         <v>2680</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="2"/>
         <v>2681</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="2"/>
         <v>2682</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="2"/>
         <v>2683</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="2"/>
         <v>2684</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>2685</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>2686</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>2687</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>2688</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>2689</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>2691</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>2692</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>2693</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>2694</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>2695</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>2696</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>2697</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>2698</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>2699</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>2700</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>2701</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>2702</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>2703</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>2704</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>2705</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>2706</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>2707</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>2708</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>2709</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>2710</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>2711</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>2712</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>2713</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>2714</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>2715</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>2716</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>2717</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>2718</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170">
         <f t="shared" si="2"/>
         <v>2719</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171">
         <f t="shared" si="2"/>
         <v>2720</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172">
         <f t="shared" si="2"/>
         <v>2721</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173">
         <f t="shared" si="2"/>
         <v>2722</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174">
         <f t="shared" si="2"/>
         <v>2723</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175">
         <f t="shared" si="2"/>
         <v>2724</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176">
         <f t="shared" si="2"/>
         <v>2725</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177">
         <f t="shared" si="2"/>
         <v>2726</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178">
         <f t="shared" si="2"/>
         <v>2727</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179">
         <f t="shared" si="2"/>
         <v>2728</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180">
         <f t="shared" si="2"/>
         <v>2729</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181">
         <f t="shared" si="2"/>
         <v>2730</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182">
         <f t="shared" si="2"/>
         <v>2731</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183">
         <f t="shared" si="2"/>
         <v>2732</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184">
         <f t="shared" si="2"/>
         <v>2733</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185">
         <f t="shared" si="2"/>
         <v>2734</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186">
         <f t="shared" si="2"/>
         <v>2735</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187">
         <f t="shared" si="2"/>
         <v>2736</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188">
         <f t="shared" si="2"/>
         <v>2737</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>2738</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>2739</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>2740</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>2741</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>2742</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>2743</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195">
         <f t="shared" ref="A195:A258" si="3">A194+1</f>
         <v>2744</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196">
         <f t="shared" si="3"/>
         <v>2745</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197">
         <f t="shared" si="3"/>
         <v>2746</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198">
         <f t="shared" si="3"/>
         <v>2747</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199">
         <f t="shared" si="3"/>
         <v>2748</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200">
         <f t="shared" si="3"/>
         <v>2749</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201">
         <f t="shared" si="3"/>
         <v>2750</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202">
         <f t="shared" si="3"/>
         <v>2751</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203">
         <f t="shared" si="3"/>
         <v>2752</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204">
         <f t="shared" si="3"/>
         <v>2753</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205">
         <f t="shared" si="3"/>
         <v>2754</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206">
         <f t="shared" si="3"/>
         <v>2755</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207">
         <f t="shared" si="3"/>
         <v>2756</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208">
         <f t="shared" si="3"/>
         <v>2757</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209">
         <f t="shared" si="3"/>
         <v>2758</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210">
         <f t="shared" si="3"/>
         <v>2759</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211">
         <f t="shared" si="3"/>
         <v>2760</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212">
         <f t="shared" si="3"/>
         <v>2761</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213">
         <f t="shared" si="3"/>
         <v>2762</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214">
         <f t="shared" si="3"/>
         <v>2763</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215">
         <f t="shared" si="3"/>
         <v>2764</v>
       </c>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216">
         <f t="shared" si="3"/>
         <v>2765</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217">
         <f t="shared" si="3"/>
         <v>2766</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218">
         <f t="shared" si="3"/>
         <v>2767</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219">
         <f t="shared" si="3"/>
         <v>2768</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220">
         <f t="shared" si="3"/>
         <v>2769</v>
       </c>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221">
         <f t="shared" si="3"/>
         <v>2770</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222">
         <f t="shared" si="3"/>
         <v>2771</v>
       </c>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223">
         <f t="shared" si="3"/>
         <v>2772</v>
       </c>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224">
         <f t="shared" si="3"/>
         <v>2773</v>
       </c>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225">
         <f t="shared" si="3"/>
         <v>2774</v>
       </c>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226">
         <f t="shared" si="3"/>
         <v>2775</v>
       </c>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227">
         <f t="shared" si="3"/>
         <v>2776</v>
       </c>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228">
         <f t="shared" si="3"/>
         <v>2777</v>
       </c>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229">
         <f t="shared" si="3"/>
         <v>2778</v>
       </c>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230">
         <f t="shared" si="3"/>
         <v>2779</v>
       </c>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231">
         <f t="shared" si="3"/>
         <v>2780</v>
       </c>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232">
         <f t="shared" si="3"/>
         <v>2781</v>
       </c>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233">
         <f t="shared" si="3"/>
         <v>2782</v>
       </c>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234">
         <f t="shared" si="3"/>
         <v>2783</v>
       </c>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235">
         <f t="shared" si="3"/>
         <v>2784</v>
       </c>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236">
         <f t="shared" si="3"/>
         <v>2785</v>
       </c>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237">
         <f t="shared" si="3"/>
         <v>2786</v>
       </c>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238">
         <f t="shared" si="3"/>
         <v>2787</v>
       </c>
     </row>
-    <row r="239" spans="1:1">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239">
         <f t="shared" si="3"/>
         <v>2788</v>
       </c>
     </row>
-    <row r="240" spans="1:1">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240">
         <f t="shared" si="3"/>
         <v>2789</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="242" spans="1:4">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242">
         <f t="shared" si="3"/>
         <v>2791</v>
       </c>
     </row>
-    <row r="243" spans="1:4">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243">
         <f t="shared" si="3"/>
         <v>2792</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244">
         <f t="shared" si="3"/>
         <v>2793</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245">
         <f t="shared" si="3"/>
         <v>2794</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246">
         <f t="shared" si="3"/>
         <v>2795</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247">
         <f t="shared" si="3"/>
         <v>2796</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248">
         <f t="shared" si="3"/>
         <v>2797</v>
       </c>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249">
         <f t="shared" si="3"/>
         <v>2798</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250">
         <f t="shared" si="3"/>
         <v>2799</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251">
         <f t="shared" si="3"/>
         <v>2800</v>
       </c>
     </row>
-    <row r="252" spans="1:4">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252">
         <f t="shared" si="3"/>
         <v>2801</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253">
         <f t="shared" si="3"/>
         <v>2802</v>
       </c>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254">
         <f t="shared" si="3"/>
         <v>2803</v>
       </c>
     </row>
-    <row r="255" spans="1:4">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255">
         <f t="shared" si="3"/>
         <v>2804</v>
       </c>
     </row>
-    <row r="256" spans="1:4">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256">
         <f t="shared" si="3"/>
         <v>2805</v>
@@ -2935,94 +2941,85 @@
         <v>51</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257">
         <f t="shared" si="3"/>
         <v>2806</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258">
         <f t="shared" si="3"/>
         <v>2807</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259">
         <f t="shared" ref="A259:A322" si="4">A258+1</f>
         <v>2808</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260">
         <f t="shared" si="4"/>
         <v>2809</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261">
         <f t="shared" si="4"/>
         <v>2810</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262">
         <f t="shared" si="4"/>
         <v>2811</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263">
         <f t="shared" si="4"/>
         <v>2812</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264">
         <f t="shared" si="4"/>
         <v>2813</v>
       </c>
     </row>
-    <row r="265" spans="1:4">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265">
         <f t="shared" si="4"/>
         <v>2814</v>
       </c>
     </row>
-    <row r="266" spans="1:4">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266">
         <f t="shared" si="4"/>
         <v>2815</v>
       </c>
     </row>
-    <row r="267" spans="1:4">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267">
         <f t="shared" si="4"/>
         <v>2816</v>
       </c>
     </row>
-    <row r="268" spans="1:4">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268">
         <f t="shared" si="4"/>
         <v>2817</v>
       </c>
     </row>
-    <row r="269" spans="1:4">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269">
         <f t="shared" si="4"/>
         <v>2818</v>
       </c>
-      <c r="B269" t="s">
-        <v>52</v>
-      </c>
-      <c r="C269" t="s">
-        <v>53</v>
-      </c>
-      <c r="D269" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4">
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270">
         <f t="shared" si="4"/>
         <v>2819</v>
@@ -3037,7 +3034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="271" spans="1:4">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271">
         <f t="shared" si="4"/>
         <v>2820</v>
@@ -3052,7 +3049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:4">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272">
         <f t="shared" si="4"/>
         <v>2821</v>
@@ -3067,7 +3064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="273" spans="1:4">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273">
         <f t="shared" si="4"/>
         <v>2822</v>
@@ -3082,94 +3079,85 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274">
         <f t="shared" si="4"/>
         <v>2823</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275">
         <f t="shared" si="4"/>
         <v>2824</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276">
         <f t="shared" si="4"/>
         <v>2825</v>
       </c>
     </row>
-    <row r="277" spans="1:4">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277">
         <f t="shared" si="4"/>
         <v>2826</v>
       </c>
     </row>
-    <row r="278" spans="1:4">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278">
         <f t="shared" si="4"/>
         <v>2827</v>
       </c>
     </row>
-    <row r="279" spans="1:4">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279">
         <f t="shared" si="4"/>
         <v>2828</v>
       </c>
     </row>
-    <row r="280" spans="1:4">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280">
         <f t="shared" si="4"/>
         <v>2829</v>
       </c>
     </row>
-    <row r="281" spans="1:4">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281">
         <f t="shared" si="4"/>
         <v>2830</v>
       </c>
     </row>
-    <row r="282" spans="1:4">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282">
         <f t="shared" si="4"/>
         <v>2831</v>
       </c>
     </row>
-    <row r="283" spans="1:4">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283">
         <f t="shared" si="4"/>
         <v>2832</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284">
         <f t="shared" si="4"/>
         <v>2833</v>
       </c>
     </row>
-    <row r="285" spans="1:4">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285">
         <f t="shared" si="4"/>
         <v>2834</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286">
         <f t="shared" si="4"/>
         <v>2835</v>
       </c>
-      <c r="B286" t="s">
-        <v>52</v>
-      </c>
-      <c r="C286" t="s">
-        <v>59</v>
-      </c>
-      <c r="D286" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4">
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287">
         <f t="shared" si="4"/>
         <v>2836</v>
@@ -3184,7 +3172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288">
         <f t="shared" si="4"/>
         <v>2837</v>
@@ -3199,7 +3187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289">
         <f t="shared" si="4"/>
         <v>2838</v>
@@ -3214,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290">
         <f t="shared" si="4"/>
         <v>2839</v>
@@ -3229,7 +3217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291">
         <f t="shared" si="4"/>
         <v>2840</v>
@@ -3247,7 +3235,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292">
         <f t="shared" si="4"/>
         <v>2841</v>
@@ -3262,7 +3250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293">
         <f t="shared" si="4"/>
         <v>2842</v>
@@ -3277,7 +3265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294">
         <f t="shared" si="4"/>
         <v>2843</v>
@@ -3292,7 +3280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295">
         <f t="shared" si="4"/>
         <v>2844</v>
@@ -3304,25 +3292,25 @@
         <v>69</v>
       </c>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296">
         <f t="shared" si="4"/>
         <v>2845</v>
       </c>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297">
         <f t="shared" si="4"/>
         <v>2846</v>
       </c>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298">
         <f t="shared" si="4"/>
         <v>2847</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299">
         <f t="shared" si="4"/>
         <v>2848</v>
@@ -3337,7 +3325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300">
         <f t="shared" si="4"/>
         <v>2849</v>
@@ -3352,7 +3340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="301" spans="1:5">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301">
         <f t="shared" si="4"/>
         <v>2850</v>
@@ -3367,7 +3355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302">
         <f t="shared" si="4"/>
         <v>2851</v>
@@ -3382,7 +3370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303">
         <f t="shared" si="4"/>
         <v>2852</v>
@@ -3397,13 +3385,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="304" spans="1:5">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304">
         <f t="shared" si="4"/>
         <v>2853</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305">
         <f t="shared" si="4"/>
         <v>2854</v>
@@ -3418,7 +3406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306">
         <f t="shared" si="4"/>
         <v>2855</v>
@@ -3433,7 +3421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307">
         <f t="shared" si="4"/>
         <v>2856</v>
@@ -3448,7 +3436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308">
         <f t="shared" si="4"/>
         <v>2857</v>
@@ -3463,7 +3451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309">
         <f t="shared" si="4"/>
         <v>2858</v>
@@ -3478,7 +3466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310">
         <f t="shared" si="4"/>
         <v>2859</v>
@@ -3493,7 +3481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311">
         <f t="shared" si="4"/>
         <v>2860</v>
@@ -3508,7 +3496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312">
         <f t="shared" si="4"/>
         <v>2861</v>
@@ -3523,7 +3511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313">
         <f t="shared" si="4"/>
         <v>2862</v>
@@ -3538,7 +3526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314">
         <f t="shared" si="4"/>
         <v>2863</v>
@@ -3553,7 +3541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315">
         <f t="shared" si="4"/>
         <v>2864</v>
@@ -3568,7 +3556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="316" spans="1:4">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316">
         <f t="shared" si="4"/>
         <v>2865</v>
@@ -3583,7 +3571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="317" spans="1:4">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317">
         <f t="shared" si="4"/>
         <v>2866</v>
@@ -3598,73 +3586,55 @@
         <v>12</v>
       </c>
     </row>
-    <row r="318" spans="1:4">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318">
         <f t="shared" si="4"/>
         <v>2867</v>
       </c>
     </row>
-    <row r="319" spans="1:4">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319">
         <f t="shared" si="4"/>
         <v>2868</v>
       </c>
-      <c r="B319" t="s">
-        <v>52</v>
-      </c>
-      <c r="C319" t="s">
-        <v>88</v>
-      </c>
-      <c r="D319" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4">
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320">
         <f t="shared" si="4"/>
         <v>2869</v>
       </c>
     </row>
-    <row r="321" spans="1:4">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321">
         <f t="shared" si="4"/>
         <v>2870</v>
       </c>
     </row>
-    <row r="322" spans="1:4">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322">
         <f t="shared" si="4"/>
         <v>2871</v>
       </c>
     </row>
-    <row r="323" spans="1:4">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323">
         <f t="shared" ref="A323:A386" si="5">A322+1</f>
         <v>2872</v>
       </c>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324">
         <f t="shared" si="5"/>
         <v>2873</v>
       </c>
     </row>
-    <row r="325" spans="1:4">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325">
         <f t="shared" si="5"/>
         <v>2874</v>
       </c>
-      <c r="B325" t="s">
-        <v>52</v>
-      </c>
-      <c r="C325" t="s">
-        <v>89</v>
-      </c>
-      <c r="D325" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4">
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326">
         <f t="shared" si="5"/>
         <v>2875</v>
@@ -3679,7 +3649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327">
         <f t="shared" si="5"/>
         <v>2876</v>
@@ -3694,7 +3664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="328" spans="1:4">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328">
         <f t="shared" si="5"/>
         <v>2877</v>
@@ -3709,46 +3679,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="329" spans="1:4">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329">
         <f t="shared" si="5"/>
         <v>2878</v>
       </c>
     </row>
-    <row r="330" spans="1:4">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330">
         <f t="shared" si="5"/>
         <v>2879</v>
       </c>
     </row>
-    <row r="331" spans="1:4">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331">
         <f t="shared" si="5"/>
         <v>2880</v>
       </c>
     </row>
-    <row r="332" spans="1:4">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332">
         <f t="shared" si="5"/>
         <v>2881</v>
       </c>
     </row>
-    <row r="333" spans="1:4">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333">
         <f t="shared" si="5"/>
         <v>2882</v>
       </c>
-      <c r="B333" t="s">
-        <v>52</v>
-      </c>
-      <c r="C333" t="s">
-        <v>93</v>
-      </c>
-      <c r="D333" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="334" spans="1:4">
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334">
         <f t="shared" si="5"/>
         <v>2883</v>
@@ -3763,7 +3724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:4">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335">
         <f t="shared" si="5"/>
         <v>2884</v>
@@ -3778,7 +3739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336">
         <f t="shared" si="5"/>
         <v>2885</v>
@@ -3787,7 +3748,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337">
         <f t="shared" si="5"/>
         <v>2886</v>
@@ -3796,7 +3757,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338">
         <f t="shared" si="5"/>
         <v>2887</v>
@@ -3805,67 +3766,58 @@
         <v>96</v>
       </c>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339">
         <f t="shared" si="5"/>
         <v>2888</v>
       </c>
     </row>
-    <row r="340" spans="1:4">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340">
         <f t="shared" si="5"/>
         <v>2889</v>
       </c>
     </row>
-    <row r="341" spans="1:4">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341">
         <f t="shared" si="5"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342">
         <f t="shared" si="5"/>
         <v>2891</v>
       </c>
     </row>
-    <row r="343" spans="1:4">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343">
         <f t="shared" si="5"/>
         <v>2892</v>
       </c>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344">
         <f t="shared" si="5"/>
         <v>2893</v>
       </c>
-      <c r="B344" t="s">
-        <v>52</v>
-      </c>
-      <c r="C344" t="s">
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <f t="shared" si="5"/>
+        <v>2894</v>
+      </c>
+      <c r="B345" t="s">
+        <v>52</v>
+      </c>
+      <c r="C345" t="s">
         <v>97</v>
       </c>
-      <c r="D344" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4">
-      <c r="A345">
-        <f t="shared" si="5"/>
-        <v>2894</v>
-      </c>
-      <c r="B345" t="s">
-        <v>52</v>
-      </c>
-      <c r="C345" t="s">
-        <v>98</v>
-      </c>
       <c r="D345" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:4">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346">
         <f t="shared" si="5"/>
         <v>2895</v>
@@ -3880,7 +3832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="347" spans="1:4">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347">
         <f t="shared" si="5"/>
         <v>2896</v>
@@ -3895,7 +3847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348">
         <f t="shared" si="5"/>
         <v>2897</v>
@@ -3910,7 +3862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:4">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349">
         <f t="shared" si="5"/>
         <v>2898</v>
@@ -3925,7 +3877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="350" spans="1:4">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350">
         <f t="shared" si="5"/>
         <v>2899</v>
@@ -3940,7 +3892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351">
         <f t="shared" si="5"/>
         <v>2900</v>
@@ -3951,59 +3903,53 @@
       <c r="C351" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="352" spans="1:4">
+      <c r="D351" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352">
         <f t="shared" si="5"/>
         <v>2901</v>
       </c>
     </row>
-    <row r="353" spans="1:5">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353">
         <f t="shared" si="5"/>
         <v>2902</v>
       </c>
     </row>
-    <row r="354" spans="1:5">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354">
         <f t="shared" si="5"/>
         <v>2903</v>
       </c>
     </row>
-    <row r="355" spans="1:5">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355">
         <f t="shared" si="5"/>
         <v>2904</v>
       </c>
     </row>
-    <row r="356" spans="1:5">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356">
         <f t="shared" si="5"/>
         <v>2905</v>
       </c>
     </row>
-    <row r="357" spans="1:5">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357">
         <f t="shared" si="5"/>
         <v>2906</v>
       </c>
     </row>
-    <row r="358" spans="1:5">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358">
         <f t="shared" si="5"/>
         <v>2907</v>
       </c>
-      <c r="B358" t="s">
-        <v>52</v>
-      </c>
-      <c r="C358" t="s">
-        <v>105</v>
-      </c>
-      <c r="D358" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="359" spans="1:5">
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359">
         <f t="shared" si="5"/>
         <v>2908</v>
@@ -4018,7 +3964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="360" spans="1:5">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360">
         <f t="shared" si="5"/>
         <v>2909</v>
@@ -4033,7 +3979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:5">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361">
         <f t="shared" si="5"/>
         <v>2910</v>
@@ -4048,7 +3994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="362" spans="1:5">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362">
         <f t="shared" si="5"/>
         <v>2911</v>
@@ -4060,49 +4006,43 @@
         <v>109</v>
       </c>
     </row>
-    <row r="363" spans="1:5">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363">
         <f t="shared" si="5"/>
         <v>2912</v>
       </c>
     </row>
-    <row r="364" spans="1:5">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364">
         <f t="shared" si="5"/>
         <v>2913</v>
       </c>
     </row>
-    <row r="365" spans="1:5">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365">
         <f t="shared" si="5"/>
         <v>2914</v>
       </c>
     </row>
-    <row r="366" spans="1:5">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366">
         <f t="shared" si="5"/>
         <v>2915</v>
       </c>
     </row>
-    <row r="367" spans="1:5">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367">
         <f t="shared" si="5"/>
         <v>2916</v>
       </c>
     </row>
-    <row r="368" spans="1:5">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368">
         <f t="shared" si="5"/>
         <v>2917</v>
       </c>
-      <c r="D368" t="s">
-        <v>12</v>
-      </c>
-      <c r="E368" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="369" spans="1:4">
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A369">
         <f t="shared" si="5"/>
         <v>2918</v>
@@ -4116,8 +4056,11 @@
       <c r="D369" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="370" spans="1:4">
+      <c r="E369" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A370">
         <f t="shared" si="5"/>
         <v>2919</v>
@@ -4132,7 +4075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A371">
         <f t="shared" si="5"/>
         <v>2920</v>
@@ -4141,43 +4084,25 @@
         <v>52</v>
       </c>
       <c r="C371" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D371" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:4">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A372">
         <f t="shared" si="5"/>
         <v>2921</v>
       </c>
-      <c r="B372" t="s">
-        <v>52</v>
-      </c>
-      <c r="C372" t="s">
-        <v>114</v>
-      </c>
-      <c r="D372" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="373" spans="1:4">
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A373">
         <f t="shared" si="5"/>
         <v>2922</v>
       </c>
-      <c r="B373" t="s">
-        <v>52</v>
-      </c>
-      <c r="C373" t="s">
-        <v>115</v>
-      </c>
-      <c r="D373" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="374" spans="1:4">
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A374">
         <f t="shared" si="5"/>
         <v>2923</v>
@@ -4192,7 +4117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="375" spans="1:4">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A375">
         <f t="shared" si="5"/>
         <v>2924</v>
@@ -4207,7 +4132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="376" spans="1:4">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A376">
         <f t="shared" si="5"/>
         <v>2925</v>
@@ -4222,22 +4147,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:4">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A377">
         <f t="shared" si="5"/>
         <v>2926</v>
       </c>
-      <c r="B377" t="s">
-        <v>52</v>
-      </c>
-      <c r="C377" t="s">
-        <v>119</v>
-      </c>
-      <c r="D377" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="378" spans="1:4">
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A378">
         <f t="shared" si="5"/>
         <v>2927</v>
@@ -4252,124 +4168,106 @@
         <v>12</v>
       </c>
     </row>
-    <row r="379" spans="1:4">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A379">
         <f t="shared" si="5"/>
         <v>2928</v>
       </c>
-      <c r="B379" t="s">
-        <v>52</v>
-      </c>
-      <c r="C379" t="s">
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <f t="shared" si="5"/>
+        <v>2929</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <f t="shared" si="5"/>
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <f t="shared" si="5"/>
+        <v>2931</v>
+      </c>
+      <c r="B382" t="s">
+        <v>52</v>
+      </c>
+      <c r="C382" t="s">
         <v>121</v>
       </c>
-      <c r="D379" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="380" spans="1:4">
-      <c r="A380">
-        <f t="shared" si="5"/>
-        <v>2929</v>
-      </c>
-      <c r="B380" t="s">
-        <v>52</v>
-      </c>
-      <c r="C380" t="s">
+      <c r="D382" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <f t="shared" si="5"/>
+        <v>2932</v>
+      </c>
+      <c r="B383" t="s">
+        <v>52</v>
+      </c>
+      <c r="C383" t="s">
         <v>122</v>
       </c>
-      <c r="D380" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="381" spans="1:4">
-      <c r="A381">
-        <f t="shared" si="5"/>
-        <v>2930</v>
-      </c>
-      <c r="B381" t="s">
-        <v>52</v>
-      </c>
-      <c r="C381" t="s">
-        <v>123</v>
-      </c>
-      <c r="D381" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="382" spans="1:4">
-      <c r="A382">
-        <f t="shared" si="5"/>
-        <v>2931</v>
-      </c>
-      <c r="B382" t="s">
-        <v>52</v>
-      </c>
-      <c r="C382" t="s">
+      <c r="D383" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <f t="shared" si="5"/>
+        <v>2933</v>
+      </c>
+      <c r="B384" t="s">
+        <v>52</v>
+      </c>
+      <c r="C384" t="s">
         <v>124</v>
       </c>
-      <c r="D382" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="383" spans="1:4">
-      <c r="A383">
-        <f t="shared" si="5"/>
-        <v>2932</v>
-      </c>
-    </row>
-    <row r="384" spans="1:4">
-      <c r="A384">
-        <f t="shared" si="5"/>
-        <v>2933</v>
-      </c>
-    </row>
-    <row r="385" spans="1:5">
+      <c r="D384" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A385">
         <f t="shared" si="5"/>
         <v>2934</v>
       </c>
     </row>
-    <row r="386" spans="1:5">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A386">
         <f t="shared" si="5"/>
         <v>2935</v>
       </c>
     </row>
-    <row r="387" spans="1:5">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A387">
         <f t="shared" ref="A387:A400" si="6">A386+1</f>
         <v>2936</v>
       </c>
     </row>
-    <row r="388" spans="1:5">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A388">
         <f t="shared" si="6"/>
         <v>2937</v>
       </c>
     </row>
-    <row r="389" spans="1:5">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A389">
         <f t="shared" si="6"/>
         <v>2938</v>
       </c>
     </row>
-    <row r="390" spans="1:5">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A390">
         <f t="shared" si="6"/>
         <v>2939</v>
       </c>
-      <c r="B390" t="s">
-        <v>52</v>
-      </c>
-      <c r="C390" t="s">
-        <v>125</v>
-      </c>
-      <c r="D390" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="391" spans="1:5">
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A391">
         <f t="shared" si="6"/>
         <v>2940</v>
@@ -4384,7 +4282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="392" spans="1:5">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A392">
         <f t="shared" si="6"/>
         <v>2941</v>
@@ -4399,7 +4297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="393" spans="1:5">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A393">
         <f t="shared" si="6"/>
         <v>2942</v>
@@ -4414,7 +4312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:5">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A394">
         <f t="shared" si="6"/>
         <v>2943</v>
@@ -4423,25 +4321,25 @@
         <v>129</v>
       </c>
     </row>
-    <row r="395" spans="1:5">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A395">
         <f t="shared" si="6"/>
         <v>2944</v>
       </c>
     </row>
-    <row r="396" spans="1:5">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A396">
         <f t="shared" si="6"/>
         <v>2945</v>
       </c>
     </row>
-    <row r="397" spans="1:5">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A397">
         <f t="shared" si="6"/>
         <v>2946</v>
       </c>
     </row>
-    <row r="398" spans="1:5">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A398">
         <f t="shared" si="6"/>
         <v>2947</v>
@@ -4450,7 +4348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:5">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A399">
         <f t="shared" si="6"/>
         <v>2948</v>
@@ -4465,7 +4363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="400" spans="1:5">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A400">
         <f t="shared" si="6"/>
         <v>2949</v>
@@ -4485,15 +4383,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17525603-7B01-ED4B-8465-45B422C7775B}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>'SID Allocation'!A327+1</f>
         <v>2877</v>
@@ -4508,9 +4409,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f>A1+1</f>
+        <f t="shared" ref="A2:A12" si="0">A1+1</f>
         <v>2878</v>
       </c>
       <c r="B2" t="s">
@@ -4520,9 +4421,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" si="0"/>
         <v>2879</v>
       </c>
       <c r="B3" t="s">
@@ -4532,9 +4433,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>2880</v>
       </c>
       <c r="B4" t="s">
@@ -4544,9 +4445,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>2881</v>
       </c>
       <c r="B5" t="s">
@@ -4556,9 +4457,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>2882</v>
       </c>
       <c r="B6" t="s">
@@ -4568,9 +4469,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>2883</v>
       </c>
       <c r="B7" t="s">
@@ -4580,9 +4481,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>2884</v>
       </c>
       <c r="B8" t="s">
@@ -4592,9 +4493,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>2885</v>
       </c>
       <c r="B9" t="s">
@@ -4604,9 +4505,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>2886</v>
       </c>
       <c r="B10" t="s">
@@ -4616,9 +4517,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>2887</v>
       </c>
       <c r="B11" t="s">
@@ -4628,9 +4529,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>2888</v>
       </c>
       <c r="B12" t="s">
@@ -4640,7 +4541,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <f>'SID Allocation'!A343+1</f>
         <v>2893</v>
@@ -4652,9 +4553,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" ref="A15:A21" si="1">A14+1</f>
         <v>2894</v>
       </c>
       <c r="B15" t="s">
@@ -4664,9 +4565,9 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="1"/>
         <v>2895</v>
       </c>
       <c r="B16" t="s">
@@ -4676,9 +4577,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="1"/>
         <v>2896</v>
       </c>
       <c r="B17" t="s">
@@ -4688,9 +4589,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="1"/>
         <v>2897</v>
       </c>
       <c r="B18" t="s">
@@ -4700,9 +4601,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="1"/>
         <v>2898</v>
       </c>
       <c r="B19" t="s">
@@ -4712,9 +4613,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="1"/>
         <v>2899</v>
       </c>
       <c r="B20" t="s">
@@ -4724,9 +4625,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="1"/>
         <v>2900</v>
       </c>
       <c r="B21" t="s">
@@ -4734,6 +4635,141 @@
       </c>
       <c r="C21" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>